<commit_message>
fix: changed the allocations
</commit_message>
<xml_diff>
--- a/SNS tokenomics tool.xlsx
+++ b/SNS tokenomics tool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\v1ctor\projects\neuralarena-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6B9CA2-2DC4-438F-92B3-2C7286C951D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3770CC-0E76-4366-BC59-46DECF2FEDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SNS configuration" sheetId="4" r:id="rId1"/>
@@ -1231,19 +1231,19 @@
                 <c:formatCode>#,##0.0;\(#,##0.0\)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.6</c:v>
+                  <c:v>4.0265486725663715</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.399999999999999</c:v>
+                  <c:v>30.973451327433629</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1756,13 +1756,13 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.9237548235310522E-2</c:v>
+                  <c:v>5.213765190462076E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.44289392121865939</c:v>
+                  <c:v>0.44418801933749646</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2236,6 +2236,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1899-440F-ACC8-8BB1C8FC383C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2369,13 +2374,13 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.9237548235310522E-2</c:v>
+                  <c:v>5.213765190462076E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4978685305460302</c:v>
+                  <c:v>0.50367432875788276</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.44289392121865939</c:v>
+                  <c:v>0.44418801933749646</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3563,7 +3568,7 @@
                 <c:formatCode>#,##0;\(#,##0\)</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20000000</c:v>
+                  <c:v>35000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3849,10 +3854,10 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>100000</c:v>
+                  <c:v>165000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>500000</c:v>
+                  <c:v>565000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3954,10 +3959,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.08</c:v>
+                  <c:v>7.5428571428571428E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4</c:v>
+                  <c:v>0.25828571428571429</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6077,7 +6082,7 @@
   </sheetPr>
   <dimension ref="A1:F1009"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
@@ -6572,14 +6577,14 @@
         <v>108</v>
       </c>
       <c r="C27" s="71">
-        <v>20000000</v>
+        <v>35000000</v>
       </c>
       <c r="D27" s="66" t="s">
         <v>61</v>
       </c>
       <c r="E27" s="67">
         <f t="shared" ref="E27:E32" si="3">C27*10^8</f>
-        <v>2000000000000000</v>
+        <v>3500000000000000</v>
       </c>
       <c r="F27" s="66" t="s">
         <v>90</v>
@@ -6593,14 +6598,14 @@
         <v>110</v>
       </c>
       <c r="C28" s="71">
-        <v>20000000</v>
+        <v>35000000</v>
       </c>
       <c r="D28" s="66" t="s">
         <v>61</v>
       </c>
       <c r="E28" s="67">
         <f t="shared" si="3"/>
-        <v>2000000000000000</v>
+        <v>3500000000000000</v>
       </c>
       <c r="F28" s="66" t="s">
         <v>90</v>
@@ -6614,14 +6619,14 @@
         <v>112</v>
       </c>
       <c r="C29" s="72">
-        <v>17000000</v>
+        <v>30000000</v>
       </c>
       <c r="D29" s="73" t="s">
         <v>61</v>
       </c>
       <c r="E29" s="74">
         <f t="shared" si="3"/>
-        <v>1700000000000000</v>
+        <v>3000000000000000</v>
       </c>
       <c r="F29" s="73" t="s">
         <v>90</v>
@@ -6677,14 +6682,14 @@
         <v>118</v>
       </c>
       <c r="C32" s="71">
-        <v>63000000</v>
+        <v>35000000</v>
       </c>
       <c r="D32" s="66" t="s">
         <v>61</v>
       </c>
       <c r="E32" s="67">
         <f t="shared" si="3"/>
-        <v>6300000000000000</v>
+        <v>3500000000000000</v>
       </c>
       <c r="F32" s="66" t="s">
         <v>90</v>
@@ -9762,8 +9767,8 @@
   </sheetPr>
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9853,7 +9858,7 @@
       </c>
       <c r="B7" s="13">
         <f>'SNS configuration'!C25*1/'Token price range'!C6 / 10^6</f>
-        <v>2.6</v>
+        <v>4.0265486725663715</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -9873,7 +9878,7 @@
       </c>
       <c r="B8" s="14">
         <f>'SNS configuration'!C28/10^6</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -9893,7 +9898,7 @@
       </c>
       <c r="B9" s="13">
         <f>B8-B7</f>
-        <v>17.399999999999999</v>
+        <v>30.973451327433629</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -9980,7 +9985,7 @@
       </c>
       <c r="B12" s="18">
         <f>B7</f>
-        <v>2.6</v>
+        <v>4.0265486725663715</v>
       </c>
       <c r="C12" s="19">
         <f>'SNS configuration'!B38</f>
@@ -9988,7 +9993,7 @@
       </c>
       <c r="D12" s="20">
         <f t="shared" ref="D12:D19" si="0">B12*C12</f>
-        <v>2.2285714285714286</v>
+        <v>3.4513274336283182</v>
       </c>
       <c r="E12" s="21">
         <f>'SNS configuration'!C38</f>
@@ -10003,11 +10008,11 @@
       </c>
       <c r="H12" s="20">
         <f t="shared" ref="H12:H14" si="2">D12*F12*G12</f>
-        <v>2.2773214285714287</v>
+        <v>3.5268252212389379</v>
       </c>
       <c r="I12" s="22">
         <f t="shared" ref="I12:I19" si="3">H12/$H$20</f>
-        <v>5.9237548235310522E-2</v>
+        <v>5.213765190462076E-2</v>
       </c>
       <c r="J12" s="19">
         <f>IF( 'SNS configuration'!$B$45, 'SNS configuration'!B50, 100%)</f>
@@ -10015,11 +10020,11 @@
       </c>
       <c r="K12" s="20">
         <f t="shared" ref="K12:K14" si="4">H12*J12</f>
-        <v>2.2773214285714287</v>
+        <v>3.5268252212389379</v>
       </c>
       <c r="L12" s="23">
         <f t="shared" ref="L12:L19" si="5">K12/$K$20</f>
-        <v>5.9237548235310522E-2</v>
+        <v>5.213765190462076E-2</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
@@ -10076,7 +10081,7 @@
       </c>
       <c r="B14" s="18">
         <f>IF('SNS configuration'!B45, 'SNS configuration'!B46*B9, 0)</f>
-        <v>17.399999999999999</v>
+        <v>30.973451327433629</v>
       </c>
       <c r="C14" s="19">
         <f>'SNS configuration'!B47</f>
@@ -10084,7 +10089,7 @@
       </c>
       <c r="D14" s="20">
         <f t="shared" si="0"/>
-        <v>17.399999999999999</v>
+        <v>30.973451327433629</v>
       </c>
       <c r="E14" s="7">
         <f>'SNS configuration'!B48</f>
@@ -10099,11 +10104,11 @@
       </c>
       <c r="H14" s="20">
         <f t="shared" si="2"/>
-        <v>19.14</v>
+        <v>34.070796460176993</v>
       </c>
       <c r="I14" s="22">
         <f t="shared" si="3"/>
-        <v>0.4978685305460302</v>
+        <v>0.50367432875788276</v>
       </c>
       <c r="J14" s="19">
         <f>IF( 'SNS configuration'!$B$45, 'SNS configuration'!B52, 100%)</f>
@@ -10111,11 +10116,11 @@
       </c>
       <c r="K14" s="20">
         <f t="shared" si="4"/>
-        <v>19.14</v>
+        <v>34.070796460176993</v>
       </c>
       <c r="L14" s="23">
         <f t="shared" si="5"/>
-        <v>0.4978685305460302</v>
+        <v>0.50367432875788276</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
@@ -10154,7 +10159,7 @@
       </c>
       <c r="B16" s="18">
         <f>'SNS configuration'!C29/10^6</f>
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C16" s="19">
         <f>'SNS configuration'!B40</f>
@@ -10162,7 +10167,7 @@
       </c>
       <c r="D16" s="20">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E16" s="21">
         <f>'SNS configuration'!C40</f>
@@ -10178,11 +10183,11 @@
       </c>
       <c r="H16" s="20">
         <f t="shared" ref="H16:H18" si="7">D16*F16*G16</f>
-        <v>17.026562499999997</v>
+        <v>30.046874999999996</v>
       </c>
       <c r="I16" s="22">
         <f t="shared" si="3"/>
-        <v>0.44289392121865939</v>
+        <v>0.44418801933749646</v>
       </c>
       <c r="J16" s="19">
         <f>IF( 'SNS configuration'!$B$45, 'SNS configuration'!B52, 100%)</f>
@@ -10190,11 +10195,11 @@
       </c>
       <c r="K16" s="20">
         <f t="shared" ref="K16:K18" si="8">H16*J16</f>
-        <v>17.026562499999997</v>
+        <v>30.046874999999996</v>
       </c>
       <c r="L16" s="23">
         <f t="shared" si="5"/>
-        <v>0.44289392121865939</v>
+        <v>0.44418801933749646</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -10300,7 +10305,7 @@
       </c>
       <c r="B19" s="18">
         <f>'SNS configuration'!C32/10^6</f>
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="C19" s="19">
         <v>0</v>
@@ -10335,14 +10340,14 @@
       <c r="C20" s="7"/>
       <c r="D20" s="20">
         <f>SUM(D12:D19)</f>
-        <v>36.628571428571426</v>
+        <v>64.424778761061944</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="20">
         <f>SUM(H12:H19)</f>
-        <v>38.443883928571424</v>
+        <v>67.64449668141593</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7">
@@ -10351,7 +10356,7 @@
       </c>
       <c r="K20" s="20">
         <f>SUM(K12:K19)</f>
-        <v>38.443883928571424</v>
+        <v>67.64449668141593</v>
       </c>
       <c r="L20" s="24"/>
     </row>
@@ -10817,8 +10822,8 @@
   </sheetPr>
   <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10853,16 +10858,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <f>'SNS configuration'!C18</f>
-        <v>100000</v>
+        <f>'SNS configuration'!C18+'SNS configuration'!C25</f>
+        <v>165000</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" ref="C5:C6" si="0">B5/$B$7</f>
-        <v>5.0000000000000001E-3</v>
+        <v>4.7142857142857143E-3</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" ref="D5:D6" si="1">C5*$B$2</f>
-        <v>0.08</v>
+        <v>7.5428571428571428E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -10870,16 +10875,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <f>'SNS configuration'!C19</f>
-        <v>500000</v>
+        <f>'SNS configuration'!C19+'SNS configuration'!C25</f>
+        <v>565000</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <v>1.6142857142857143E-2</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.25828571428571429</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -10888,7 +10893,7 @@
       </c>
       <c r="B7" s="5">
         <f>'SNS configuration'!C28</f>
-        <v>20000000</v>
+        <v>35000000</v>
       </c>
       <c r="D7" s="6">
         <f>D11</f>
@@ -10920,7 +10925,7 @@
       </c>
       <c r="B32" s="7">
         <f>B31/'Token price range'!C6</f>
-        <v>40</v>
+        <v>61.946902654867259</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -10947,7 +10952,7 @@
       </c>
       <c r="B35" s="7">
         <f>B32/B33-B34</f>
-        <v>5.6142857142857148</v>
+        <v>8.7495575221238937</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -10970,6 +10975,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>